<commit_message>
Fixing criteria file award names
</commit_message>
<xml_diff>
--- a/Awards_2019_Parsing.xlsx
+++ b/Awards_2019_Parsing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arsalan/dev/maxgala/awards-nomination-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4623DE14-0019-BE4F-83DE-D06A8FF231AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1356BD-CA40-2841-A6DB-F144EE1D5BE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67720" yWindow="7100" windowWidth="21880" windowHeight="20600" activeTab="2" xr2:uid="{6DFFBB05-D152-4EC9-A6DA-8A7E4E1A2A67}"/>
+    <workbookView xWindow="67720" yWindow="7100" windowWidth="21880" windowHeight="20600" activeTab="1" xr2:uid="{6DFFBB05-D152-4EC9-A6DA-8A7E4E1A2A67}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="96">
   <si>
     <t>Column</t>
   </si>
@@ -49,13 +49,7 @@
     <t>Charity of the Year</t>
   </si>
   <si>
-    <t>Entrepreneur Of The Year</t>
-  </si>
-  <si>
     <t>Friend Of The Community</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Professional Excellence Award </t>
   </si>
   <si>
     <t>Woman Of The Year</t>
@@ -328,6 +322,9 @@
   </si>
   <si>
     <t>There are some fields in the form that are for users to upload files, for now put the Jotform links, we will later convert these to MAX Google Drive links where we will have access controls in place</t>
+  </si>
+  <si>
+    <t>Entrepreneur Of Year</t>
   </si>
 </sst>
 </file>
@@ -802,56 +799,56 @@
   <sheetData>
     <row r="1" spans="1:2" ht="31" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="192" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -867,9 +864,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D73C98-F194-4106-A136-41AA21C8A308}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -893,552 +890,552 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235064C6-C200-4972-B534-F2DB84043511}">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
@@ -1470,112 +1467,112 @@
   <sheetData>
     <row r="1" spans="1:36" ht="350" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="M1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="AD1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="AJ1" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
@@ -1583,7 +1580,7 @@
         <v>43538.933032407411</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
@@ -1599,7 +1596,7 @@
         <v>43536.38721064815</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
@@ -1607,7 +1604,7 @@
         <v>43536.015115740738</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">

</xml_diff>